<commit_message>
Arreglos en Anteproyecto. Gantt, cronograma, requerimientos
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="170">
   <si>
     <t>Tarea</t>
   </si>
@@ -450,27 +450,6 @@
     <t>RF-15.1 Notificación de trabajo aceptado</t>
   </si>
   <si>
-    <t>RF-16.1 Agregar y Quitar de Favoritos un prestador de servicio</t>
-  </si>
-  <si>
-    <t>RF-17.1 Visualizar Favoritos</t>
-  </si>
-  <si>
-    <t>RF-18.1 Visualizar puntuación y comentarios</t>
-  </si>
-  <si>
-    <t>RF-19.1 Recuperación de contraseña</t>
-  </si>
-  <si>
-    <t>RF-20.1 Agregar y Quitar de Amigos</t>
-  </si>
-  <si>
-    <t>RF-21.1 Denunciar Publicación/Postulación/Usuario</t>
-  </si>
-  <si>
-    <t>RF-22.2 Idenificar mejor oferta de la publicación</t>
-  </si>
-  <si>
     <t>1.5.1</t>
   </si>
   <si>
@@ -498,12 +477,6 @@
     <t>1.5.9</t>
   </si>
   <si>
-    <t>1.5.10</t>
-  </si>
-  <si>
-    <t>1.5.11</t>
-  </si>
-  <si>
     <t>1.5.12</t>
   </si>
   <si>
@@ -567,10 +540,34 @@
     <t>VER ESTE SPRINT CAPAZ QUE ES MUCHO</t>
   </si>
   <si>
-    <t>CAPAZ CONVIENE PASAR HORAS AL SPRINT 5 Y 6</t>
-  </si>
-  <si>
     <t>1.5.20</t>
+  </si>
+  <si>
+    <t>1.4.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF-10.2 Aprobación de oferta laboral </t>
+  </si>
+  <si>
+    <t>RF-16.1 Visualizar puntuación y comentarios</t>
+  </si>
+  <si>
+    <t>RF-17.1 Recuperación de contraseña</t>
+  </si>
+  <si>
+    <t>RF18.1 Posibilidad de ingreso con Facebook</t>
+  </si>
+  <si>
+    <t>RF-19.1 Denunciar Publicación/Postulación/Usuario</t>
+  </si>
+  <si>
+    <t>RF-20.2 Idenificar mejor oferta de la publicación</t>
+  </si>
+  <si>
+    <t>Arreglos en base a devolución</t>
+  </si>
+  <si>
+    <t>Promedio de 40 horas semanales</t>
   </si>
 </sst>
 </file>
@@ -987,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F110"/>
+  <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="B100" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,7 +1024,8 @@
         <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>720</v>
+        <f>SUM(C3+C30+C47+C67+C87+C108)</f>
+        <v>795</v>
       </c>
       <c r="D2" s="3">
         <v>42860</v>
@@ -1044,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D3" s="5">
         <v>42860</v>
@@ -1053,7 +1051,7 @@
         <v>42886</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1077,7 +1075,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1090,7 +1088,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1103,7 +1101,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1370,79 +1368,77 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8">
-        <f>SUM(C4:C27)</f>
-        <v>135</v>
+      <c r="B28" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="8">
+        <f>SUM(C4:C28)</f>
+        <v>150</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="4">
-        <v>75</v>
-      </c>
-      <c r="D29" s="5">
+      <c r="C30" s="4">
+        <v>85</v>
+      </c>
+      <c r="D30" s="5">
         <v>42887</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E30" s="5">
         <v>42901</v>
       </c>
-      <c r="F29" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="2">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="F30" s="9" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C32" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C33" s="2">
         <v>3</v>
@@ -1452,476 +1448,472 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>20</v>
+        <v>60</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C34" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C35" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C36" s="2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="2">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="C40" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="2"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="8">
-        <f>SUM(C30:C43)</f>
-        <v>75</v>
+      <c r="A44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="2">
+        <v>10</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="4">
-        <v>115</v>
-      </c>
-      <c r="D45" s="5">
-        <v>42902</v>
-      </c>
-      <c r="E45" s="5">
-        <v>42924</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="2">
+        <v>10</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="2">
-        <v>3</v>
+      <c r="A46" s="2"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="8">
+        <f>SUM(C31:C45)</f>
+        <v>85</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" s="2">
-        <v>5</v>
-      </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="A47" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="4">
+        <v>130</v>
+      </c>
+      <c r="D47" s="5">
+        <v>42902</v>
+      </c>
+      <c r="E47" s="5">
+        <v>42924</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C49" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>20</v>
+        <v>85</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C50" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>45</v>
+        <v>86</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C51" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>77</v>
+        <v>87</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C52" s="2">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="10" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>78</v>
+        <v>88</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C53" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="2">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
+      <c r="F54" s="10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C55" s="2">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C56" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C57" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C58" s="2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="C59" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="C60" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C61" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C62" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2"/>
-      <c r="B63" s="7"/>
+      <c r="A63" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="C63" s="2">
-        <f>SUM(C46:C62)</f>
-        <v>115</v>
+        <v>2</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C64" s="4">
-        <v>115</v>
-      </c>
-      <c r="D64" s="5">
-        <v>42925</v>
-      </c>
-      <c r="E64" s="5">
-        <v>42947</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="A64" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C64" s="2">
+        <v>10</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="A65" s="2"/>
       <c r="B65" s="7" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="C65" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A66" s="2"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="2">
-        <v>5</v>
+        <f>SUM(C48:C65)</f>
+        <v>130</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C67" s="2">
-        <v>4</v>
-      </c>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="A67" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C67" s="4">
+        <v>130</v>
+      </c>
+      <c r="D67" s="5">
+        <v>42925</v>
+      </c>
+      <c r="E67" s="5">
+        <v>42947</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C68" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>20</v>
+        <v>110</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C69" s="2">
         <v>5</v>
@@ -1931,547 +1923,593 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>45</v>
+        <v>111</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C70" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>103</v>
+        <v>18</v>
       </c>
       <c r="C71" s="2">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>104</v>
+        <v>113</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="C72" s="2">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-      <c r="F72" s="10" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C73" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C74" s="2">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="C75" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C76" s="2">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
+      <c r="F76" s="10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="C77" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="C78" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="C79" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="C80" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" s="2"/>
-      <c r="B81" s="7"/>
+      <c r="A81" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="C81" s="2">
-        <f>SUM(C65:C80)</f>
-        <v>115</v>
+        <v>4</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C82" s="4">
-        <v>140</v>
-      </c>
-      <c r="D82" s="5">
-        <v>42948</v>
-      </c>
-      <c r="E82" s="5">
-        <v>42975</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="A82" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C82" s="2">
+        <v>3</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C83" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C84" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
-        <v>139</v>
-      </c>
+      <c r="A85" s="2"/>
       <c r="B85" s="7" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="C85" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="A86" s="2"/>
+      <c r="B86" s="7"/>
       <c r="C86" s="2">
-        <v>5</v>
+        <f>SUM(C68:C85)</f>
+        <v>130</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C87" s="2">
-        <v>4</v>
-      </c>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="A87" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="4">
+        <v>150</v>
+      </c>
+      <c r="D87" s="5">
+        <v>42948</v>
+      </c>
+      <c r="E87" s="5">
+        <v>42973</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B88" s="6" t="s">
-        <v>45</v>
+        <v>130</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C88" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B89" s="6" t="s">
-        <v>127</v>
+        <v>131</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C89" s="2">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C90" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
-      <c r="F90" s="10" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C91" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>130</v>
+        <v>20</v>
       </c>
       <c r="C92" s="2">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="C93" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C94" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C95" s="2">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
+      <c r="F95" s="10"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C96" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C97" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="C98" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B99" s="7" t="s">
-        <v>49</v>
+        <v>141</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="C99" s="2">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>50</v>
+        <v>142</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="C100" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B101" s="7" t="s">
-        <v>51</v>
+        <v>143</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="C101" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C102" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" s="2"/>
-      <c r="B103" s="7"/>
+      <c r="A103" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="C103" s="2">
-        <f>SUM(C83:C102)</f>
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C104" s="4">
-        <v>140</v>
-      </c>
-      <c r="D104" s="5">
-        <v>42976</v>
-      </c>
-      <c r="E104" s="5">
-        <v>43003</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>167</v>
-      </c>
+      <c r="A104" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="2">
+        <v>2</v>
+      </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B105" s="6" t="s">
-        <v>158</v>
+        <v>160</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="C105" s="2">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>159</v>
+      <c r="A106" s="2"/>
+      <c r="B106" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="C106" s="2">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B107" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="A107" s="2"/>
+      <c r="B107" s="7"/>
       <c r="C107" s="2">
-        <v>15</v>
+        <f>SUM(C88:C106)</f>
+        <v>150</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C108" s="2">
-        <v>3</v>
-      </c>
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
+      <c r="A108" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C108" s="4">
+        <v>150</v>
+      </c>
+      <c r="D108" s="5">
+        <v>42974</v>
+      </c>
+      <c r="E108" s="5">
+        <v>43003</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C109" s="2">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" s="2"/>
-      <c r="B110" s="6"/>
+      <c r="A110" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="C110" s="2">
-        <f>SUM(C105:C109)</f>
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C111" s="2">
+        <v>15</v>
+      </c>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C112" s="2">
+        <v>3</v>
+      </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C113" s="2">
+        <v>32</v>
+      </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A114" s="2"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="2">
+        <f>SUM(C109:C113)</f>
+        <v>150</v>
+      </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Avanzando con el MER
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\Documentación Proyecto\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -708,8 +703,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -976,7 +999,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -986,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B101" sqref="B101"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Más de la documentación
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 4" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="225">
   <si>
     <t>Tarea</t>
   </si>
@@ -563,13 +565,178 @@
   </si>
   <si>
     <t>RF-20.2 Identificar mejor oferta de la publicación</t>
+  </si>
+  <si>
+    <t>Horas estimadas</t>
+  </si>
+  <si>
+    <t>Horas reales</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>COMPLETADA</t>
+  </si>
+  <si>
+    <t>Se efectuó una reunión a fin de planificar los pasos a seguir en cada tarea.</t>
+  </si>
+  <si>
+    <t>Se realizó una idea inicial del MER y el diagrama de clases necesarios para el manejo de usuarios.</t>
+  </si>
+  <si>
+    <t>Se completó la parte del MER que corresponde a la pila de este sprint.</t>
+  </si>
+  <si>
+    <t>Se completó la parte del diagrama de clases que corresponde a la pila de este sprint.</t>
+  </si>
+  <si>
+    <t>Se realizó el script para crear la base de datos correspondiente a la pila del sprint.</t>
+  </si>
+  <si>
+    <t>Se crearon las pruebas unitarias en el backend para los métodos a realizar en esta pila del sprint.</t>
+  </si>
+  <si>
+    <t>PARCIALMENTE COMPLETADA</t>
+  </si>
+  <si>
+    <t>Si bien se llegó a lo que se pretendía (que un administrador pueda cambiar su password y el de los demás usuarios), optamos por investigar más adelante sobre cómo realizar envíos de emails y así poder resetear uno mismo su contraseña de ser necesario.</t>
+  </si>
+  <si>
+    <t>Se realizó el backend que permite el alta de usuarios de tipo cliente al sistema, así como el frontend que le permite a cualquier persona no registrada, registrarse en el mismo.</t>
+  </si>
+  <si>
+    <t>Se realizó el backend que permite específicamente la modificación de la contraseña de los usuarios, así como el frontend que permite realizar la misma acción.</t>
+  </si>
+  <si>
+    <t>Se realizó el backend que permite la modificación de datos de los usuarios de tipo cliente, así como el frontend que permite realizar la misma acción.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan ver un listado de todos los clientes registrados en el sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan habilitar y deshabilitar a los clientes registrados en el sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan ingresar nuevos usuarios de tipo administrador al sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir la modificación de datos de los usuarios de tipo administrador.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan ver un listado de todos los administradores del sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan habilitar y deshabilitar a los administradores del sistema.</t>
+  </si>
+  <si>
+    <t>ELIMINADA</t>
+  </si>
+  <si>
+    <t>Se realizó el ingreso en la base de datos. El script que crea la base, da de alta un usuario super administrador para cada integrante del equipo.</t>
+  </si>
+  <si>
+    <t>Si bien se llegó a lo que se pretendía (que los usuarios puedan acceder al sistema una vez logueados, y que de no estarlo tengas acceso limitado a las diferentes pantallas), optamos por investigar más adelante sobre el protocolo OAuth, a fin de realizar un sistema más seguro y que cuente con controles extra sobre si el usuario que está realizando una acción posee permisos para hacerlo.</t>
+  </si>
+  <si>
+    <t>Se realizaron pruebas en el backend y frontend, a fin de validar que no ocurran problemas al ingresar datos no esperados y demás.</t>
+  </si>
+  <si>
+    <t>Se realizaron las 2 reuniones pactadas con el tutor.</t>
+  </si>
+  <si>
+    <t>Se realizó la documentación correspondiente al sprint.</t>
+  </si>
+  <si>
+    <t>1.1.25</t>
+  </si>
+  <si>
+    <t>1.1.26</t>
+  </si>
+  <si>
+    <t>Reunión con los Grupos Foco para entrega del sprint</t>
+  </si>
+  <si>
+    <t>Se realizaron reuniones con los grupos focos que simulan a los usuarios de tipo Cliente y Administrador.</t>
+  </si>
+  <si>
+    <t>Tras la presentación del frontend al grupo foco que simula a los usuarios de tipo cliente, encontraron problemas con el diseño responsivo de la aplicación. Se corrigieron los detalles. El grupo foco de los usuarios administradores no realizó aportes que requieran cambios.</t>
+  </si>
+  <si>
+    <t>Investigación sobre API's REST</t>
+  </si>
+  <si>
+    <t>1.1.27</t>
+  </si>
+  <si>
+    <t>1.1.28</t>
+  </si>
+  <si>
+    <t>Investigación sobre subida de imágenes mediante API's REST</t>
+  </si>
+  <si>
+    <t>Se optó por agregarle una foto de perfil a los usuarios, momento en el que nos encontramos con el problema de pasar las imágenes por servicios web. Tenemos la idea de evitar pasarla convertida a Base64 a fin de no convertir el servicio que se encargue de ello en uno sumamente lento.</t>
+  </si>
+  <si>
+    <t>El equipo decidió no realizar los casos de uso para las tareas de complejidad baja y media/baja, contando así con tiempo extra para dedicarle a otras tareas.</t>
+  </si>
+  <si>
+    <t>Se instaló el software necesario en las PC's de todos los integrantes y se crearon los proyectos.</t>
+  </si>
+  <si>
+    <t>El grupo de trabajo se juntó a fin de dar un repaso a lo realizado en el sprint y sacar las conclusiones del mismo.</t>
+  </si>
+  <si>
+    <t>Se realizaron investigaciones sobre las API's REST, así como la forma en la que se generan estos servicios desde .NET. Se logró dejar un ejemplo andando a fin de continuar creando los demás a partir de la muestra.</t>
+  </si>
+  <si>
+    <t>1.2.15</t>
+  </si>
+  <si>
+    <t>1.2.16</t>
+  </si>
+  <si>
+    <t>Se realizó la reunión pacta con el tutor.</t>
+  </si>
+  <si>
+    <t>Tras la presentación de los avances a los grupos, no suergieron detalles a corregir con respecto a las tareas presentadas.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan dar de alta nuevos servicios.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan modificar los servicios existentes.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan visualizar un listado con todos los servicios existentes.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan habilitar o deshabilitar los servicios existentes.</t>
+  </si>
+  <si>
+    <t>1.2.17</t>
+  </si>
+  <si>
+    <t>1.2.18</t>
+  </si>
+  <si>
+    <t>POSTERGADA</t>
+  </si>
+  <si>
+    <t>La tarea se realizará en el Sprint 5</t>
+  </si>
+  <si>
+    <t>Investigación sobre protocolo OAuth.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -607,8 +774,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +820,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -673,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -699,6 +880,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -999,7 +1219,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1009,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,4 +2759,1013 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D2:D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.77734375" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11">
+        <v>2</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
+        <v>5</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="11">
+        <v>6</v>
+      </c>
+      <c r="D4" s="11">
+        <v>10</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="11">
+        <v>10</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="11">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11">
+        <v>4</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="11">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11">
+        <v>3</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>3</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="11">
+        <v>7</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11">
+        <v>5</v>
+      </c>
+      <c r="D12" s="11">
+        <v>4</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11">
+        <v>9</v>
+      </c>
+      <c r="D13" s="11">
+        <v>4</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11">
+        <v>4</v>
+      </c>
+      <c r="D14" s="11">
+        <v>3</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="11">
+        <v>5</v>
+      </c>
+      <c r="D15" s="11">
+        <v>4</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11">
+        <v>6</v>
+      </c>
+      <c r="D16" s="11">
+        <v>4</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="11">
+        <v>4</v>
+      </c>
+      <c r="D17" s="11">
+        <v>3</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="11">
+        <v>4</v>
+      </c>
+      <c r="D18" s="11">
+        <v>2</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="11">
+        <v>4</v>
+      </c>
+      <c r="D19" s="11">
+        <v>3</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="11">
+        <v>4</v>
+      </c>
+      <c r="D20" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="11">
+        <v>8</v>
+      </c>
+      <c r="D21" s="11">
+        <v>8</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="11">
+        <v>5</v>
+      </c>
+      <c r="D22" s="11">
+        <v>5</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="11">
+        <v>3</v>
+      </c>
+      <c r="D23" s="11">
+        <v>4</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="11">
+        <v>2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="11">
+        <v>10</v>
+      </c>
+      <c r="D25" s="11">
+        <v>8</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" s="11">
+        <v>2</v>
+      </c>
+      <c r="D26" s="11">
+        <v>2</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" s="11">
+        <v>10</v>
+      </c>
+      <c r="D27" s="11">
+        <v>4</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="20">
+        <v>10</v>
+      </c>
+      <c r="D28" s="20">
+        <v>15</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C29" s="20">
+        <v>10</v>
+      </c>
+      <c r="D29" s="20">
+        <v>15</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="23" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.77734375" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="11">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="11">
+        <v>5</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11">
+        <v>3</v>
+      </c>
+      <c r="D4" s="11">
+        <v>6</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="11">
+        <v>3</v>
+      </c>
+      <c r="D5" s="11">
+        <v>6</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="11">
+        <v>5</v>
+      </c>
+      <c r="D7" s="11">
+        <v>7</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="11">
+        <v>16</v>
+      </c>
+      <c r="D8" s="11">
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="11">
+        <v>7</v>
+      </c>
+      <c r="D9" s="11">
+        <v>6</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="11">
+        <v>6</v>
+      </c>
+      <c r="D10" s="11">
+        <v>4</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="11">
+        <v>5</v>
+      </c>
+      <c r="D11" s="11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="11">
+        <v>4</v>
+      </c>
+      <c r="D12" s="11">
+        <v>4</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="11">
+        <v>3</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="11">
+        <v>10</v>
+      </c>
+      <c r="D15" s="11">
+        <v>9</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C16" s="11">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="11">
+        <v>10</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C18" s="20">
+        <v>10</v>
+      </c>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="20">
+        <v>10</v>
+      </c>
+      <c r="D19" s="20">
+        <v>0</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Listado de servicios habilitados desde angular quedó pronto. Para poder ver las imagenes se deben correr los dos proyectos a la vez en el visual. FALTÓ SELECCIÓN DE CATEGORIAS EN LAS PREGUNTAS DE LOS SERVICIOS ES OPCIONAL, POR EL MOMENTO SE CREAN TODAS CON TAEGORÍA 1
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Github\ProyectoFinal\Documentacion\Documentación Proyecto\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Sprint 4" sheetId="3" r:id="rId3"/>
     <sheet name="Sprint 5" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +32,7 @@
     <author>Usuario</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -706,12 +711,6 @@
     <t>Tras la presentación de los avances a los grupos, no suergieron detalles a corregir con respecto a las tareas presentadas.</t>
   </si>
   <si>
-    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan dar de alta nuevos servicios.</t>
-  </si>
-  <si>
-    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan modificar los servicios existentes.</t>
-  </si>
-  <si>
     <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan visualizar un listado con todos los servicios existentes.</t>
   </si>
   <si>
@@ -755,6 +754,12 @@
   </si>
   <si>
     <t>1.5.22</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan dar de alta nuevos servicios.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan modificar los servicios existentes.</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1243,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2132,7 +2137,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>200</v>
@@ -2145,7 +2150,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>167</v>
@@ -2403,7 +2408,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>200</v>
@@ -2416,7 +2421,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>167</v>
@@ -2685,7 +2690,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>200</v>
@@ -2698,7 +2703,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>167</v>
@@ -3411,8 +3416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3566,7 +3571,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>67</v>
       </c>
@@ -3583,10 +3588,10 @@
         <v>174</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>68</v>
       </c>
@@ -3603,7 +3608,7 @@
         <v>174</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3623,7 +3628,7 @@
         <v>174</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3643,7 +3648,7 @@
         <v>174</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3768,10 +3773,10 @@
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C18" s="15">
         <v>10</v>
@@ -3780,15 +3785,15 @@
         <v>0</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>206</v>
@@ -3800,10 +3805,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3815,7 +3820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -4150,7 +4155,7 @@
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>200</v>
@@ -4170,7 +4175,7 @@
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>167</v>
@@ -4184,10 +4189,10 @@
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C21" s="15">
         <v>10</v>
@@ -4198,7 +4203,7 @@
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
Documentación Sprint 3 y 4
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="247">
   <si>
     <t>Tarea</t>
   </si>
@@ -615,9 +615,6 @@
     <t>Se realizó el backend que permite el alta de usuarios de tipo cliente al sistema, así como el frontend que le permite a cualquier persona no registrada, registrarse en el mismo.</t>
   </si>
   <si>
-    <t>Se realizó el backend que permite específicamente la modificación de la contraseña de los usuarios, así como el frontend que permite realizar la misma acción.</t>
-  </si>
-  <si>
     <t>Se realizó el backend que permite la modificación de datos de los usuarios de tipo cliente, así como el frontend que permite realizar la misma acción.</t>
   </si>
   <si>
@@ -627,18 +624,6 @@
     <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan habilitar y deshabilitar a los clientes registrados en el sistema.</t>
   </si>
   <si>
-    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan ingresar nuevos usuarios de tipo administrador al sistema.</t>
-  </si>
-  <si>
-    <t>Se realizó todo lo necesario para permitir la modificación de datos de los usuarios de tipo administrador.</t>
-  </si>
-  <si>
-    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan ver un listado de todos los administradores del sistema.</t>
-  </si>
-  <si>
-    <t>Se realizó todo lo necesario para que los usuarios de tipo administrador y superadministrador, puedan habilitar y deshabilitar a los administradores del sistema.</t>
-  </si>
-  <si>
     <t>ELIMINADA</t>
   </si>
   <si>
@@ -705,18 +690,9 @@
     <t>1.2.16</t>
   </si>
   <si>
-    <t>Se realizó la reunión pacta con el tutor.</t>
-  </si>
-  <si>
-    <t>Tras la presentación de los avances a los grupos, no suergieron detalles a corregir con respecto a las tareas presentadas.</t>
-  </si>
-  <si>
     <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan visualizar un listado con todos los servicios existentes.</t>
   </si>
   <si>
-    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo superadministrador puedan habilitar o deshabilitar los servicios existentes.</t>
-  </si>
-  <si>
     <t>1.2.17</t>
   </si>
   <si>
@@ -756,10 +732,76 @@
     <t>1.5.22</t>
   </si>
   <si>
-    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan dar de alta nuevos servicios.</t>
-  </si>
-  <si>
     <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan modificar los servicios existentes.</t>
+  </si>
+  <si>
+    <t>RF-5.5 Alta de Pregunta</t>
+  </si>
+  <si>
+    <t>RF-5.6 Modificación de Pregunta</t>
+  </si>
+  <si>
+    <t>RF-5.7 Listado de Pregunta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se efectuó una reunión a fin de planificar los pasos a seguir en cada tarea. Se incorporaron nuevos requerimientos a realizar en el Sprint. </t>
+  </si>
+  <si>
+    <t>Se completó la parte del MER que corresponde a la pila de este Sprint.</t>
+  </si>
+  <si>
+    <t>Se crearon las pruebas unitarias en el backend para los métodos a realizar en esta pila del Sprint.</t>
+  </si>
+  <si>
+    <t>1.2.19</t>
+  </si>
+  <si>
+    <t>1.2.20</t>
+  </si>
+  <si>
+    <t>1.2.21</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan dar de alta nuevas preguntas que podrán ser asociadas a servicios al momento de su creación.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan modificar las preguntas existentes en el sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administarador y superadministrador puedan visualizar un listado con todos las preguntas existentes.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan dar de alta nuevos servicios, asociando a los mismos las preguntas que correspondan.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir que los usuarios de tipo administrador y superadministrador puedan habilitar o deshabilitar los servicios existentes.</t>
+  </si>
+  <si>
+    <t>El grupo de trabajo se reunió a fin de dar un repaso a lo realizado en el sprint y sacar las conclusiones del mismo.</t>
+  </si>
+  <si>
+    <t>Se realizó la reunión pactada con el tutor.</t>
+  </si>
+  <si>
+    <t>Se realizó la documentación correspondiente al Sprint.</t>
+  </si>
+  <si>
+    <t>Luego de la presentación de los avances a los grupos, no suergieron detalles a corregir con respecto a las tareas presentadas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realizó el backend que permite específicamente la modificación de la contraseña de los usuarios, así como el frontend que permite realizar la misma acción. Los usuarios administradores como los superAdministradores pueden cambiar la contraseña de cualquier cliente desde su interfaz, los usuarios clientes pueden cambiar su propia contraseña desde su interfaz en angular. </t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo superadministrador, puedan ingresar nuevos usuarios de tipo administrador al sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para permitir la modificación de datos de los usuarios de tipo administrador. El usuario súper administrador puede modificar los datos de todos los administrdaores. El usuario administrador puede modificar sus datos.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo superadministrador, puedan ver un listado de todos los administradores del sistema.</t>
+  </si>
+  <si>
+    <t>Se realizó todo lo necesario para que los usuarios de tipo superadministrador, puedan habilitar y deshabilitar a los administradores del sistema.</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1637,10 +1679,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1650,7 +1692,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>167</v>
@@ -1866,10 +1908,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
@@ -1879,7 +1921,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>167</v>
@@ -2137,10 +2179,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C65" s="1">
         <v>3</v>
@@ -2150,7 +2192,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>167</v>
@@ -2408,10 +2450,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C85" s="1">
         <v>4</v>
@@ -2421,7 +2463,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>167</v>
@@ -2690,10 +2732,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C106" s="1">
         <v>4</v>
@@ -2703,7 +2745,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>167</v>
@@ -2811,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2883,7 +2925,7 @@
         <v>174</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2920,10 +2962,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3043,10 +3085,10 @@
         <v>174</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
@@ -3063,7 +3105,7 @@
         <v>174</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>184</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3083,7 +3125,7 @@
         <v>174</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3103,10 +3145,10 @@
         <v>174</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>39</v>
       </c>
@@ -3123,10 +3165,10 @@
         <v>174</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>40</v>
       </c>
@@ -3143,7 +3185,7 @@
         <v>174</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>189</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3183,10 +3225,10 @@
         <v>174</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
@@ -3203,7 +3245,7 @@
         <v>174</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3223,7 +3265,7 @@
         <v>174</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3243,7 +3285,7 @@
         <v>181</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3263,7 +3305,7 @@
         <v>174</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -3283,7 +3325,7 @@
         <v>174</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3303,7 +3345,7 @@
         <v>174</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3323,15 +3365,15 @@
         <v>174</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C26" s="6">
         <v>2</v>
@@ -3343,12 +3385,12 @@
         <v>174</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>167</v>
@@ -3363,15 +3405,15 @@
         <v>174</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C28" s="15">
         <v>10</v>
@@ -3383,15 +3425,15 @@
         <v>174</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C29" s="15">
         <v>10</v>
@@ -3403,7 +3445,7 @@
         <v>181</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3414,10 +3456,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3451,7 +3493,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>57</v>
       </c>
@@ -3468,7 +3510,7 @@
         <v>174</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>175</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3485,10 +3527,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3508,7 +3550,7 @@
         <v>174</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3568,27 +3610,27 @@
         <v>174</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>63</v>
+        <v>224</v>
       </c>
       <c r="C8" s="6">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D8" s="6">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3596,19 +3638,19 @@
         <v>68</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>64</v>
+        <v>225</v>
       </c>
       <c r="C9" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3616,199 +3658,259 @@
         <v>69</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>65</v>
+        <v>226</v>
       </c>
       <c r="C10" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C11" s="6">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="C12" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C13" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D13" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>73</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C14" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>74</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D15" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>174</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6">
+        <v>3</v>
+      </c>
+      <c r="D16" s="6">
+        <v>3</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6">
+        <v>9</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="6">
+        <v>10</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C21" s="15">
+        <v>10</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="C16" s="6">
-        <v>2</v>
-      </c>
-      <c r="D16" s="6">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" s="12" t="s">
+      <c r="F21" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="C22" s="15">
+        <v>10</v>
+      </c>
+      <c r="D22" s="15">
+        <v>0</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>213</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="6">
-        <v>10</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="C18" s="15">
-        <v>10</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C19" s="15">
-        <v>10</v>
-      </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -3889,10 +3991,10 @@
         <v>0</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4090,7 +4192,7 @@
         <v>174</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4110,7 +4212,7 @@
         <v>174</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4130,7 +4232,7 @@
         <v>174</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4150,15 +4252,15 @@
         <v>174</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C19" s="6">
         <v>3</v>
@@ -4170,12 +4272,12 @@
         <v>174</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>167</v>
@@ -4189,10 +4291,10 @@
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C21" s="15">
         <v>10</v>
@@ -4203,10 +4305,10 @@
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C22" s="15">
         <v>10</v>

</xml_diff>

<commit_message>
Segundo informe de avances
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -4,14 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="627" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 3" sheetId="2" r:id="rId2"/>
     <sheet name="Replanificación S4" sheetId="5" r:id="rId3"/>
     <sheet name="Sprint 4" sheetId="3" r:id="rId4"/>
-    <sheet name="Sprint 5" sheetId="4" r:id="rId5"/>
+    <sheet name="Replanificación S5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sprint 5" sheetId="4" r:id="rId6"/>
+    <sheet name="Replanificación S6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="216">
   <si>
     <t>Tarea</t>
   </si>
@@ -572,45 +574,6 @@
     <t>Horas estimadas</t>
   </si>
   <si>
-    <t>Horas reales</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>COMPLETADA</t>
-  </si>
-  <si>
-    <t>Se efectuó una reunión a fin de planificar los pasos a seguir en cada tarea.</t>
-  </si>
-  <si>
-    <t>Se completó la parte del MER que corresponde a la pila de este sprint.</t>
-  </si>
-  <si>
-    <t>Se completó la parte del diagrama de clases que corresponde a la pila de este sprint.</t>
-  </si>
-  <si>
-    <t>Se realizó el script para crear la base de datos correspondiente a la pila del sprint.</t>
-  </si>
-  <si>
-    <t>Se crearon las pruebas unitarias en el backend para los métodos a realizar en esta pila del sprint.</t>
-  </si>
-  <si>
-    <t>ELIMINADA</t>
-  </si>
-  <si>
-    <t>Se realizaron pruebas en el backend y frontend, a fin de validar que no ocurran problemas al ingresar datos no esperados y demás.</t>
-  </si>
-  <si>
-    <t>Se realizaron las 2 reuniones pactadas con el tutor.</t>
-  </si>
-  <si>
-    <t>Se realizó la documentación correspondiente al sprint.</t>
-  </si>
-  <si>
     <t>1.1.25</t>
   </si>
   <si>
@@ -620,9 +583,6 @@
     <t>Reunión con los Grupos Foco para entrega del sprint</t>
   </si>
   <si>
-    <t>Se realizaron reuniones con los grupos focos que simulan a los usuarios de tipo Cliente y Administrador.</t>
-  </si>
-  <si>
     <t>Investigación sobre API's REST</t>
   </si>
   <si>
@@ -635,12 +595,6 @@
     <t>Investigación sobre subida de imágenes mediante API's REST</t>
   </si>
   <si>
-    <t>El equipo decidió no realizar los casos de uso para las tareas de complejidad baja y media/baja, contando así con tiempo extra para dedicarle a otras tareas.</t>
-  </si>
-  <si>
-    <t>El grupo de trabajo se juntó a fin de dar un repaso a lo realizado en el sprint y sacar las conclusiones del mismo.</t>
-  </si>
-  <si>
     <t>1.2.15</t>
   </si>
   <si>
@@ -668,9 +622,6 @@
     <t>1.3.20</t>
   </si>
   <si>
-    <t>1.3.21</t>
-  </si>
-  <si>
     <t>1.4.18</t>
   </si>
   <si>
@@ -695,9 +646,6 @@
     <t>1.2.19</t>
   </si>
   <si>
-    <t>1.2.20</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -714,6 +662,51 @@
   </si>
   <si>
     <t>No surgieron detalles a corregir</t>
+  </si>
+  <si>
+    <t>La tarea se realizará en el Sprint 6</t>
+  </si>
+  <si>
+    <t>Alta de preguntas en la base de datos.</t>
+  </si>
+  <si>
+    <t>Investigación sobre autenticación y autorización</t>
+  </si>
+  <si>
+    <t>Investigación e implementación de la subida de imágenes mediante API's REST</t>
+  </si>
+  <si>
+    <t>RF-6.1 Publicación de oferta de servicio</t>
+  </si>
+  <si>
+    <t>RF-6.2 Modificación de oferta de servicio</t>
+  </si>
+  <si>
+    <t>RF-6.3 Listado de las ofertas de servicio</t>
+  </si>
+  <si>
+    <t>RF-6.4 Habilitar/Deshabilitar publicación de oferta de servicio</t>
+  </si>
+  <si>
+    <t>RF-7.1 Listado de publicaciones de ofertas de servicio habilitadas</t>
+  </si>
+  <si>
+    <t>RF-8.1 Visualizar datos de un prestador de servicio</t>
+  </si>
+  <si>
+    <t>RF-9.1 Comentarios y puntuación de un servicio utilizado</t>
+  </si>
+  <si>
+    <t>Investigación e integración de algún módulo de Angular que permita subir el frontend a un servidor de testing</t>
+  </si>
+  <si>
+    <t>1.4.20</t>
+  </si>
+  <si>
+    <t>1.4.21</t>
+  </si>
+  <si>
+    <t>1.4.22</t>
   </si>
 </sst>
 </file>
@@ -758,7 +751,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,12 +785,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -847,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -864,9 +851,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -882,23 +866,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -914,6 +883,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -933,14 +911,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1250,7 +1225,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1260,34 +1235,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7" style="20" customWidth="1"/>
-    <col min="2" max="2" width="66.6640625" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44" style="20" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="20"/>
+    <col min="1" max="1" width="7" style="14" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44" style="14" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1326,7 +1301,7 @@
       <c r="E3" s="4">
         <v>42886</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="15" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1644,10 +1619,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -1657,7 +1632,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>167</v>
@@ -1685,7 +1660,7 @@
       <c r="E30" s="4">
         <v>42901</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="15" t="s">
         <v>168</v>
       </c>
     </row>
@@ -1873,10 +1848,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
@@ -1886,7 +1861,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>167</v>
@@ -1914,7 +1889,7 @@
       <c r="E47" s="4">
         <v>42924</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="F47" s="15" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2008,7 +1983,7 @@
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="22" t="s">
+      <c r="F54" s="16" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2144,10 +2119,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C65" s="1">
         <v>3</v>
@@ -2157,7 +2132,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>167</v>
@@ -2185,7 +2160,7 @@
       <c r="E67" s="4">
         <v>42947</v>
       </c>
-      <c r="F67" s="21" t="s">
+      <c r="F67" s="15" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2305,7 +2280,7 @@
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="22" t="s">
+      <c r="F76" s="16" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2415,10 +2390,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C85" s="1">
         <v>4</v>
@@ -2428,7 +2403,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>167</v>
@@ -2456,7 +2431,7 @@
       <c r="E87" s="4">
         <v>42973</v>
       </c>
-      <c r="F87" s="21" t="s">
+      <c r="F87" s="15" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2563,7 +2538,7 @@
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="F95" s="22"/>
+      <c r="F95" s="16"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
@@ -2697,10 +2672,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C106" s="1">
         <v>4</v>
@@ -2710,7 +2685,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>167</v>
@@ -2738,7 +2713,7 @@
       <c r="E108" s="4">
         <v>43003</v>
       </c>
-      <c r="F108" s="21" t="s">
+      <c r="F108" s="15" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2818,500 +2793,500 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="6.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="12" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>215</v>
+      <c r="D1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="23">
-        <v>3</v>
-      </c>
-      <c r="D2" s="23">
+      <c r="C2" s="17">
+        <v>3</v>
+      </c>
+      <c r="D2" s="17">
         <v>2</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="17">
         <v>10</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="17">
         <v>5</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="17">
         <v>6</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="17">
         <v>10</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="20">
         <v>10</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="20">
         <v>0</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28" t="s">
-        <v>216</v>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="23">
-        <v>3</v>
-      </c>
-      <c r="D6" s="23">
+      <c r="C6" s="17">
+        <v>3</v>
+      </c>
+      <c r="D6" s="17">
         <v>3.5</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="23">
-        <v>3</v>
-      </c>
-      <c r="D7" s="23">
-        <v>4</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="C7" s="17">
+        <v>3</v>
+      </c>
+      <c r="D7" s="17">
+        <v>4</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="17">
         <v>5</v>
       </c>
-      <c r="D8" s="23">
-        <v>3</v>
-      </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="D8" s="17">
+        <v>3</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="17">
         <v>8</v>
       </c>
-      <c r="D9" s="23">
-        <v>3</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="17">
         <v>9</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="17">
         <v>5</v>
       </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="17">
         <v>10</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="17">
         <v>7</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="17">
         <v>5</v>
       </c>
-      <c r="D12" s="23">
-        <v>4</v>
-      </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="D12" s="17">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="17">
         <v>9</v>
       </c>
-      <c r="D13" s="23">
-        <v>4</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="D13" s="17">
+        <v>4</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="23">
-        <v>4</v>
-      </c>
-      <c r="D14" s="23">
-        <v>3</v>
-      </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="C14" s="17">
+        <v>4</v>
+      </c>
+      <c r="D14" s="17">
+        <v>3</v>
+      </c>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="17">
         <v>5</v>
       </c>
-      <c r="D15" s="23">
-        <v>4</v>
-      </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="D15" s="17">
+        <v>4</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="17">
         <v>6</v>
       </c>
-      <c r="D16" s="23">
-        <v>4</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
+      <c r="D16" s="17">
+        <v>4</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="23">
-        <v>4</v>
-      </c>
-      <c r="D17" s="23">
-        <v>3</v>
-      </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
+      <c r="C17" s="17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="23">
-        <v>4</v>
-      </c>
-      <c r="D18" s="23">
+      <c r="C18" s="17">
+        <v>4</v>
+      </c>
+      <c r="D18" s="17">
         <v>2</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="23">
-        <v>4</v>
-      </c>
-      <c r="D19" s="23">
-        <v>3</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
+      <c r="C19" s="17">
+        <v>4</v>
+      </c>
+      <c r="D19" s="17">
+        <v>3</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="23">
-        <v>4</v>
-      </c>
-      <c r="D20" s="23">
+      <c r="C20" s="17">
+        <v>4</v>
+      </c>
+      <c r="D20" s="17">
         <v>0.25</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="17">
         <v>8</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="17">
         <v>8</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
     </row>
     <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="17">
         <v>5</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="17">
         <v>5</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="23">
-        <v>3</v>
-      </c>
-      <c r="D23" s="23">
-        <v>4</v>
-      </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
+      <c r="C23" s="17">
+        <v>3</v>
+      </c>
+      <c r="D23" s="17">
+        <v>4</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="17">
         <v>2</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="17">
         <v>2</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="17">
         <v>10</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="17">
         <v>8</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
     </row>
     <row r="26" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" s="23">
+      <c r="A26" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="17">
         <v>2</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="17">
         <v>2</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
     </row>
     <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B27" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="17">
         <v>10</v>
       </c>
-      <c r="D27" s="23">
-        <v>4</v>
-      </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="D27" s="17">
+        <v>4</v>
+      </c>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
     </row>
     <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="23">
+      <c r="A28" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="17">
         <v>10</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="17">
         <v>15</v>
       </c>
-      <c r="E28" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="F28" s="25"/>
+      <c r="E28" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="B29" s="30" t="s">
-        <v>191</v>
-      </c>
-      <c r="C29" s="29">
+      <c r="A29" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="23">
         <v>10</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="23">
         <v>15</v>
       </c>
-      <c r="E29" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="F29" s="31"/>
+      <c r="E29" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="25"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <v>172</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="6">
         <v>132.75</v>
       </c>
     </row>
@@ -3326,34 +3301,34 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="40" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40" style="20"/>
-    <col min="7" max="7" width="50.5546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="40" style="20"/>
+    <col min="1" max="1" width="6.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40" style="14"/>
+    <col min="7" max="7" width="50.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="40" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3497,7 +3472,7 @@
         <v>70</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C12" s="1">
         <v>10</v>
@@ -3559,10 +3534,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -3572,7 +3547,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>167</v>
@@ -3590,375 +3565,357 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="18.77734375" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="6.88671875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20" style="12" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18.77734375" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>215</v>
+      <c r="D1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="23">
-        <v>3</v>
-      </c>
-      <c r="D2" s="23">
-        <v>3</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="C2" s="17">
+        <v>3</v>
+      </c>
+      <c r="D2" s="17">
+        <v>3</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="23">
-        <v>3</v>
-      </c>
-      <c r="D3" s="23">
+      <c r="C3" s="17">
+        <v>3</v>
+      </c>
+      <c r="D3" s="17">
         <v>6</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="23">
-        <v>3</v>
-      </c>
-      <c r="D4" s="23">
+      <c r="C4" s="17">
+        <v>3</v>
+      </c>
+      <c r="D4" s="17">
         <v>6</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="23">
-        <v>4</v>
-      </c>
-      <c r="D5" s="23">
-        <v>4</v>
-      </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="C5" s="17">
+        <v>4</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="17">
         <v>5</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="17">
         <v>7</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="23">
+      <c r="C7" s="17">
         <v>16</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="17">
         <v>12</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="17">
         <v>7</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="17">
         <v>6</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="17">
         <v>6</v>
       </c>
-      <c r="D9" s="23">
-        <v>4</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="D9" s="17">
+        <v>4</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="17">
         <v>5</v>
       </c>
-      <c r="D10" s="23">
-        <v>3</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
+      <c r="D10" s="17">
+        <v>3</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" s="26">
+      <c r="B11" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="20">
         <v>10</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="20">
         <v>0</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28" t="s">
-        <v>198</v>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="23">
-        <v>4</v>
-      </c>
-      <c r="D12" s="23">
-        <v>4</v>
-      </c>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
+      <c r="C12" s="17">
+        <v>4</v>
+      </c>
+      <c r="D12" s="17">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="23">
-        <v>3</v>
-      </c>
-      <c r="D13" s="23">
-        <v>3</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
+      <c r="C13" s="17">
+        <v>3</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="17">
         <v>1</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="17">
         <v>1</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="17">
         <v>10</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="17">
         <v>9</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="17">
+        <v>2</v>
+      </c>
+      <c r="D16" s="17">
+        <v>2</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="20">
+        <v>10</v>
+      </c>
+      <c r="D17" s="20">
+        <v>0</v>
+      </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="C18" s="17">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" s="17">
+        <v>2</v>
+      </c>
+      <c r="D19" s="17">
+        <v>2</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" s="23">
-        <v>2</v>
-      </c>
-      <c r="D16" s="23">
-        <v>2</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+      <c r="B20" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="26">
-        <v>10</v>
-      </c>
-      <c r="D17" s="26">
-        <v>0</v>
-      </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>208</v>
-      </c>
-      <c r="C18" s="23">
-        <v>2</v>
-      </c>
-      <c r="D18" s="23">
-        <v>2</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="F18" s="25"/>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="C19" s="23">
-        <v>2</v>
-      </c>
-      <c r="D19" s="23">
-        <v>2</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="C20" s="23">
-        <v>1</v>
-      </c>
-      <c r="D20" s="23">
-        <v>2</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>213</v>
-      </c>
-      <c r="F20" s="25"/>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
-        <v>212</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C21" s="26">
-        <v>10</v>
-      </c>
-      <c r="D21" s="26">
-        <v>0</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="F21" s="28" t="s">
-        <v>198</v>
+      <c r="F20" s="22" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3968,402 +3925,1030 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" style="18" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.77734375" style="14" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUM(C3:C22)</f>
+        <v>125</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42902</v>
+      </c>
+      <c r="E2" s="4">
+        <v>42924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="1">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="1">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="1">
+        <v>12</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="1">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="89.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="17">
+        <v>3</v>
+      </c>
+      <c r="D2" s="17">
+        <v>3</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="17">
+        <v>4</v>
+      </c>
+      <c r="D3" s="17">
+        <v>5</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4</v>
+      </c>
+      <c r="D4" s="17">
+        <v>6</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="17">
+        <v>5</v>
+      </c>
+      <c r="D5" s="17">
+        <v>4</v>
+      </c>
+      <c r="E5" s="17"/>
+      <c r="F5" s="27"/>
+    </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="17">
+        <v>6</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="17">
+        <v>8</v>
+      </c>
+      <c r="D7" s="17">
+        <v>6</v>
+      </c>
+      <c r="E7" s="17"/>
+      <c r="F7" s="27"/>
+    </row>
+    <row r="8" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" s="17">
+        <v>5</v>
+      </c>
+      <c r="D8" s="17">
+        <v>5</v>
+      </c>
+      <c r="E8" s="17"/>
+      <c r="F8" s="27"/>
+    </row>
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>207</v>
+      </c>
+      <c r="C9" s="17">
+        <v>5</v>
+      </c>
+      <c r="D9" s="17">
+        <v>4</v>
+      </c>
+      <c r="E9" s="17"/>
+      <c r="F9" s="27"/>
+    </row>
+    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="17">
+        <v>3</v>
+      </c>
+      <c r="D10" s="17">
+        <v>3</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="17">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17">
+        <v>6</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="17">
+        <v>5</v>
+      </c>
+      <c r="D12" s="17">
+        <v>4</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="27"/>
+    </row>
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" s="17">
+        <v>12</v>
+      </c>
+      <c r="D13" s="17">
+        <v>12</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="27"/>
+    </row>
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="17">
+        <v>10</v>
+      </c>
+      <c r="D14" s="17">
+        <v>15</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>212</v>
+      </c>
+      <c r="C15" s="17">
+        <v>15</v>
+      </c>
+      <c r="D15" s="17">
+        <v>30</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="17">
+        <v>4</v>
+      </c>
+      <c r="D16" s="17">
+        <v>4</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="17">
+        <v>3</v>
+      </c>
+      <c r="D17" s="17">
+        <v>3</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="17">
+        <v>2</v>
+      </c>
+      <c r="D18" s="17">
+        <v>2</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="27"/>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="17">
+        <v>10</v>
+      </c>
+      <c r="D19" s="17">
+        <v>10</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="13" t="s">
+      <c r="C20" s="17">
+        <v>3</v>
+      </c>
+      <c r="D20" s="17">
+        <v>3</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C21" s="17">
+        <v>10</v>
+      </c>
+      <c r="D21" s="17">
+        <v>7</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUM(C3:C24)</f>
+        <v>148</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42925</v>
+      </c>
+      <c r="E2" s="4">
+        <v>42947</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="6">
-        <v>3</v>
-      </c>
-      <c r="D2" s="6">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6">
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="14"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6">
-        <v>4</v>
-      </c>
-      <c r="D4" s="6">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6">
-        <v>6</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="14"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="14"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="1">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
-        <v>4</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="6">
-        <v>6</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="1">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="1">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="1">
         <v>7</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="6">
-        <v>19</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="6">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="6">
-        <v>11</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="6">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="6">
-        <v>9</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C13" s="6">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="6">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="14"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="6">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6">
-        <v>8</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" s="13" t="s">
+      <c r="C19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="6">
-        <v>3</v>
-      </c>
-      <c r="D16" s="6">
-        <v>5</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17" s="13" t="s">
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="13" t="s">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C22" s="1">
         <v>10</v>
       </c>
-      <c r="D18" s="6">
-        <v>11</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C19" s="6">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6">
-        <v>3</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="B20" s="13" t="s">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C24" s="1">
         <v>10</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C21" s="15">
-        <v>10</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-    </row>
-    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C22" s="15">
-        <v>10</v>
-      </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
La base de la parte de seguridad está - Falta modificar el Login
</commit_message>
<xml_diff>
--- a/Documentacion/Documentación Proyecto/Cronograma.xlsx
+++ b/Documentacion/Documentación Proyecto/Cronograma.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="627" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" tabRatio="627" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Replanificación S5" sheetId="6" r:id="rId5"/>
     <sheet name="Sprint 5" sheetId="4" r:id="rId6"/>
     <sheet name="Replanificación S6" sheetId="7" r:id="rId7"/>
+    <sheet name="Sprint 6" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="221">
   <si>
     <t>Tarea</t>
   </si>
@@ -707,6 +708,21 @@
   </si>
   <si>
     <t>1.4.22</t>
+  </si>
+  <si>
+    <t>RF-10.1 Publicación de Solicitud de Servicio</t>
+  </si>
+  <si>
+    <t>RF-10.2 Aprobación de Solicitud de Servicio</t>
+  </si>
+  <si>
+    <t>RF-11.1 Listado de Solicitudes de Servicio</t>
+  </si>
+  <si>
+    <t>RF-12.1 Postulación de un Usuario Cliente en una Solicitud de Servicio</t>
+  </si>
+  <si>
+    <t>RF-12.2 Selección de un Trabajador para Realizar el trabajo publicado</t>
   </si>
 </sst>
 </file>
@@ -834,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -917,6 +933,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1225,7 +1251,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1235,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD86"/>
+    <sheetView topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3567,8 +3593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D20" sqref="D2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4245,7 +4271,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD29"/>
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4609,8 +4635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4953,4 +4979,393 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="28">
+        <v>3</v>
+      </c>
+      <c r="D2" s="28">
+        <v>3</v>
+      </c>
+      <c r="E2" s="28"/>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="28">
+        <v>4</v>
+      </c>
+      <c r="D3" s="28">
+        <v>5</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="30"/>
+    </row>
+    <row r="4" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="28">
+        <v>4</v>
+      </c>
+      <c r="D4" s="28">
+        <v>6</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="28">
+        <v>5</v>
+      </c>
+      <c r="D5" s="28">
+        <v>3</v>
+      </c>
+      <c r="E5" s="28"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="28">
+        <v>6</v>
+      </c>
+      <c r="D6" s="28">
+        <v>6</v>
+      </c>
+      <c r="E6" s="28"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="C7" s="28">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28">
+        <v>3.75</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="28">
+        <v>4</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="28">
+        <v>2</v>
+      </c>
+      <c r="D9" s="28">
+        <v>2.5</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="28">
+        <v>19</v>
+      </c>
+      <c r="D10" s="28">
+        <v>15</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C11" s="28">
+        <v>5</v>
+      </c>
+      <c r="D11" s="28">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" s="28">
+        <v>14</v>
+      </c>
+      <c r="D12" s="28">
+        <v>7</v>
+      </c>
+      <c r="E12" s="28"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="28">
+        <v>10</v>
+      </c>
+      <c r="D13" s="28">
+        <v>12</v>
+      </c>
+      <c r="E13" s="28"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="C14" s="28">
+        <v>8</v>
+      </c>
+      <c r="D14" s="28">
+        <v>8</v>
+      </c>
+      <c r="E14" s="28"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="28">
+        <v>11</v>
+      </c>
+      <c r="D15" s="28">
+        <v>10</v>
+      </c>
+      <c r="E15" s="28"/>
+      <c r="F15" s="30"/>
+    </row>
+    <row r="16" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="28">
+        <v>7</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="28">
+        <v>10</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="28">
+        <v>4</v>
+      </c>
+      <c r="D18" s="28">
+        <v>6</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="28">
+        <v>3</v>
+      </c>
+      <c r="D19" s="28">
+        <v>3</v>
+      </c>
+      <c r="E19" s="28"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="28">
+        <v>2</v>
+      </c>
+      <c r="D20" s="28">
+        <v>2</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="28">
+        <v>10</v>
+      </c>
+      <c r="D21" s="28">
+        <v>10</v>
+      </c>
+      <c r="E21" s="28"/>
+      <c r="F21" s="30"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="28">
+        <v>4</v>
+      </c>
+      <c r="D22" s="28">
+        <v>4</v>
+      </c>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="28">
+        <v>10</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>